<commit_message>
[Add] do some change
</commit_message>
<xml_diff>
--- a/C内存图.xlsx
+++ b/C内存图.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luochao/c_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yytd/luochao/github_lc/c_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1BE5A-E857-BE4B-AA9C-223986952066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="1960" windowWidth="23000" windowHeight="14240" activeTab="2"/>
+    <workbookView xWindow="21360" yWindow="6500" windowWidth="23000" windowHeight="14240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据类型的本质" sheetId="1" r:id="rId1"/>
     <sheet name="虚拟内存" sheetId="2" r:id="rId2"/>
     <sheet name="指针" sheetId="3" r:id="rId3"/>
+    <sheet name="变量的本质" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>1G（物理内存）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -202,12 +204,47 @@
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>0x11223311</t>
+  </si>
+  <si>
+    <t>0x11223311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x22222222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变量（固定内存块别名）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -232,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +410,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -422,103 +465,115 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,7 +613,7 @@
         <xdr:cNvPr id="2" name="上箭头 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9982853-A7E6-2941-ADE0-F8166D8C9DE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9982853-A7E6-2941-ADE0-F8166D8C9DE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -618,7 +673,7 @@
         <xdr:cNvPr id="3" name="上箭头 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C6C2A2F6-B83F-DB48-8B2D-79A3299B42BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C2A2F6-B83F-DB48-8B2D-79A3299B42BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -678,7 +733,7 @@
         <xdr:cNvPr id="4" name="上箭头 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{64D17A87-B8BB-FE4D-9E3C-94C2174A72DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D17A87-B8BB-FE4D-9E3C-94C2174A72DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -740,7 +795,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="右弧形箭头 5"/>
+        <xdr:cNvPr id="6" name="右弧形箭头 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -802,7 +863,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="文本框 10"/>
+        <xdr:cNvPr id="11" name="文本框 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -884,7 +951,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="左大括号 11"/>
+        <xdr:cNvPr id="12" name="左大括号 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -936,7 +1009,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="左大括号 12"/>
+        <xdr:cNvPr id="13" name="左大括号 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -988,7 +1067,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="左大括号 13"/>
+        <xdr:cNvPr id="14" name="左大括号 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1020,6 +1105,368 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文本框 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2434FC57-0D26-7645-8AF1-6E2B52A27977}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="419100"/>
+          <a:ext cx="1524000" cy="3187700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>int</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>10;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>20</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> 直接修改</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>int</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> * </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>&amp;a;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>20;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>     </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> 间接修改</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>int</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>addr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>(int)&amp;a;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>((int</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>)addr)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>200</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> 间接修改</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="上弧形箭头 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA4C8760-C046-784D-8D36-BB896934A70D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="6175375" y="1546225"/>
+          <a:ext cx="1238250" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1324,14 +1771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1339,14 +1786,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="23.83203125" style="1" customWidth="1"/>
@@ -1358,35 +1805,35 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D1" s="24" t="s">
+    <row r="1" spans="2:14">
+      <c r="D1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="J1" s="24" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="J1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-    </row>
-    <row r="2" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+    </row>
+    <row r="2" spans="2:14" ht="17" thickBot="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
@@ -1397,15 +1844,15 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="45"/>
+      <c r="K3" s="47"/>
       <c r="L3" s="6"/>
       <c r="M3" s="7"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="8"/>
@@ -1414,13 +1861,13 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="11"/>
       <c r="M4" s="12"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="8"/>
@@ -1429,13 +1876,13 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="11"/>
       <c r="M5" s="12"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="8"/>
@@ -1444,13 +1891,13 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="11"/>
       <c r="M6" s="12"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="8"/>
@@ -1459,13 +1906,13 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="11"/>
       <c r="M7" s="12"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="8"/>
@@ -1474,13 +1921,13 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="11"/>
       <c r="M8" s="12"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="8"/>
@@ -1489,13 +1936,13 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="11"/>
       <c r="M9" s="12"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="8"/>
@@ -1504,13 +1951,13 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="11"/>
       <c r="M10" s="12"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="8"/>
@@ -1519,13 +1966,13 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
       <c r="L11" s="11"/>
       <c r="M11" s="12"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="9"/>
@@ -1534,13 +1981,13 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
       <c r="L12" s="11"/>
       <c r="M12" s="12"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="9"/>
@@ -1549,13 +1996,13 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
       <c r="L13" s="11"/>
       <c r="M13" s="12"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="9"/>
@@ -1564,13 +2011,13 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="25"/>
       <c r="L14" s="11"/>
       <c r="M14" s="12"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="9"/>
@@ -1579,13 +2026,13 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
       <c r="L15" s="11"/>
       <c r="M15" s="12"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="9"/>
@@ -1594,13 +2041,13 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="11"/>
       <c r="M16" s="12"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="9"/>
@@ -1609,13 +2056,13 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="25"/>
       <c r="L17" s="11"/>
       <c r="M17" s="12"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="9"/>
@@ -1624,13 +2071,13 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="9"/>
@@ -1639,13 +2086,13 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="25"/>
       <c r="L19" s="11"/>
       <c r="M19" s="12"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="9"/>
@@ -1654,13 +2101,13 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="25"/>
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="9"/>
@@ -1669,13 +2116,13 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="25"/>
       <c r="L21" s="11"/>
       <c r="M21" s="12"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="9"/>
@@ -1684,13 +2131,13 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="25"/>
       <c r="L22" s="11"/>
       <c r="M22" s="12"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="9" t="s">
@@ -1709,7 +2156,7 @@
       <c r="M23" s="13"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" ht="17" thickBot="1">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="14" t="s">
@@ -1728,7 +2175,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1743,7 +2190,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1762,7 +2209,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" ht="17" thickBot="1">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1777,7 +2224,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="35" t="s">
@@ -1794,7 +2241,7 @@
       <c r="M28" s="37"/>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="38"/>
@@ -1809,7 +2256,7 @@
       <c r="M29" s="40"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" ht="17" thickBot="1">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="41"/>
@@ -1824,7 +2271,7 @@
       <c r="M30" s="43"/>
       <c r="N30" s="2"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1839,7 +2286,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1854,7 +2301,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
-    <row r="33" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="17" thickBot="1">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1869,7 +2316,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="26" t="s">
@@ -1886,7 +2333,7 @@
       <c r="M34" s="28"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="29"/>
@@ -1901,7 +2348,7 @@
       <c r="M35" s="31"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="29"/>
@@ -1916,7 +2363,7 @@
       <c r="M36" s="31"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="17" thickBot="1">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="32"/>
@@ -1931,7 +2378,7 @@
       <c r="M37" s="34"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1946,7 +2393,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1961,7 +2408,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2012,290 +2459,296 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="54.6640625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" style="18" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="50" t="s">
+    <row r="2" spans="2:8" ht="38" customHeight="1">
+      <c r="B2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-    </row>
-    <row r="3" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="2:8" ht="26" customHeight="1" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="23"/>
-      <c r="F3" s="47"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="47"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="47"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="48"/>
       <c r="E6" s="48"/>
-      <c r="F6" s="47"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
+    <row r="7" spans="2:8">
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="48"/>
       <c r="E7" s="48"/>
-      <c r="F7" s="47"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="47"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="48"/>
       <c r="E9" s="48"/>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="47"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="47"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
-      <c r="F13" s="47"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
-      <c r="F14" s="47"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
-      <c r="F15" s="47"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
+    <row r="16" spans="2:8">
+      <c r="B16" s="2">
+        <v>8</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
-      <c r="F16" s="47"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="47"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="47"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="47"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="19" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="47"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="47"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="47"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="47"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
+    <row r="25" spans="2:8">
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="47"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="47" t="s">
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="19" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="47"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="17" thickBot="1">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="22"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="47"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="47"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="47"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
@@ -2310,11 +2763,6 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
@@ -2322,16 +2770,148 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E04129F-37F1-5E4C-BBF3-A1A8900FBE60}">
+  <dimension ref="E3:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="51" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="51"/>
+    <col min="5" max="5" width="14.83203125" style="51" customWidth="1"/>
+    <col min="6" max="6" width="21" style="51" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="51" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="51"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:8">
+      <c r="E3" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8">
+      <c r="F4" s="52"/>
+    </row>
+    <row r="5" spans="5:8">
+      <c r="F5" s="53"/>
+    </row>
+    <row r="6" spans="5:8">
+      <c r="F6" s="53">
+        <v>10</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8">
+      <c r="F7" s="53"/>
+    </row>
+    <row r="8" spans="5:8">
+      <c r="E8" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="53"/>
+    </row>
+    <row r="9" spans="5:8">
+      <c r="F9" s="52"/>
+    </row>
+    <row r="10" spans="5:8">
+      <c r="F10" s="52"/>
+    </row>
+    <row r="11" spans="5:8">
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="5:8">
+      <c r="F12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8">
+      <c r="F13" s="54"/>
+    </row>
+    <row r="14" spans="5:8">
+      <c r="F14" s="54"/>
+    </row>
+    <row r="15" spans="5:8">
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="5:8">
+      <c r="F16" s="52"/>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="F17" s="53"/>
+    </row>
+    <row r="18" spans="5:8">
+      <c r="F18" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8">
+      <c r="F19" s="53"/>
+    </row>
+    <row r="20" spans="5:8">
+      <c r="E20" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="53"/>
+    </row>
+    <row r="21" spans="5:8">
+      <c r="F21" s="52"/>
+    </row>
+    <row r="22" spans="5:8">
+      <c r="F22" s="52"/>
+    </row>
+    <row r="23" spans="5:8">
+      <c r="F23" s="52"/>
+    </row>
+    <row r="24" spans="5:8">
+      <c r="F24" s="52"/>
+    </row>
+    <row r="25" spans="5:8">
+      <c r="F25" s="52"/>
+    </row>
+    <row r="26" spans="5:8">
+      <c r="F26" s="52"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] review C language until string_copy
</commit_message>
<xml_diff>
--- a/C内存图.xlsx
+++ b/C内存图.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yytd/luochao/github_lc/c_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1BE5A-E857-BE4B-AA9C-223986952066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E40A681-27D7-5B46-A572-E1EA8ED42F4C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="6500" windowWidth="23000" windowHeight="14240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19500" yWindow="1880" windowWidth="25200" windowHeight="16760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据类型的本质" sheetId="1" r:id="rId1"/>
     <sheet name="虚拟内存" sheetId="2" r:id="rId2"/>
     <sheet name="指针" sheetId="3" r:id="rId3"/>
     <sheet name="变量的本质" sheetId="4" r:id="rId4"/>
+    <sheet name="str++和p++、sizeof" sheetId="5" r:id="rId5"/>
+    <sheet name="字符串的内存四区图" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>1G（物理内存）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -216,10 +219,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>地址区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -237,6 +236,186 @@
   </si>
   <si>
     <t>变量（固定内存块别名）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\0'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  'c’</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常量区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"abcd"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(32位)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str1+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str1+3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p = str1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>静态区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全局区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>‘a’</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>‘\0’</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf[2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf[4]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf2[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf2[2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf2[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf2[4]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>‘b’</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全局图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>堆区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"3333"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x33333333</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"111111"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x11111111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -244,7 +423,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,8 +447,30 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +498,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +641,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -471,6 +702,90 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,76 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -561,20 +807,62 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1470,6 +1758,2409 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文本框 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA18992-62B4-0C44-B006-F54FB047E250}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="203200" y="139700"/>
+          <a:ext cx="2374900" cy="2578100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>str1[]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>{'a',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'b',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'c',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'d',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'\0'};</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>str3[128]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>{'x',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'y',</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>'z'};</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> * </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>str2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>"abcd";</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>sizeof</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>(str1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>sizeof(str2)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>4(32</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t>位</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>sizeof(str3)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+            <a:t>128</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>strlen(str1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>strlen(str2)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>strlen(str3)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>3</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="左大括号 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ECF860E-F087-0949-86E2-A6596A502934}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3822700" y="1079500"/>
+          <a:ext cx="292100" cy="863600"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="左大括号 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A03E646A-9E71-E849-A7FE-FCFF3EFB076F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="2705100"/>
+          <a:ext cx="279400" cy="1270000"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1422400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直线箭头连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A73C3120-FEDE-554E-A771-BAE54E6D1ECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5549900" y="1943100"/>
+          <a:ext cx="838200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直线箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97990D7F-FD9D-914D-9331-E65960901879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5245100" y="3975100"/>
+          <a:ext cx="1244600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="左大括号 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF8D8432-1310-6946-AEE1-E70342D54BFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3835400" y="4749800"/>
+          <a:ext cx="254000" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="文本框 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AFF98C2-9054-454B-A6A9-266C253975EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="3390900"/>
+          <a:ext cx="2489200" cy="4102100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>str1[i]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t> 和</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>++</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> 有什么区别。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>// </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en" sz="1100"/>
+            <a:t>通过</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>下标</a:t>
+          </a:r>
+          <a:endParaRPr lang="en" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>int len = strlen(str1);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>for ( i = 0; i &lt; len; i++)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>printf("%c\n", str1[i]); </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>//  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>通过指针</a:t>
+          </a:r>
+          <a:endParaRPr lang="en" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>char *p = NULL;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>p = str1;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>for ( i = 0; i &lt; len; i++, p++)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>printf("%c\n", *p);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100"/>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>p++</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 为</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 用指针遍历，需要不断的改变指针的方向，也就是需要不断的改变</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>的值，比直接用数组名索引，多一步内存的操作，理论上会慢一些。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en" altLang="zh-CN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直线箭头连接符 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4259D1B6-81EC-6D4C-856E-1FC803960D51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5600700" y="1320800"/>
+          <a:ext cx="685800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直线箭头连接符 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2643D6C-BF44-F545-812A-666711362D34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5562600" y="1739900"/>
+          <a:ext cx="825500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="文本框 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A047AA3-C2CB-F040-8434-C15AEC2D0691}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6464300" y="114300"/>
+          <a:ext cx="1803400" cy="1003300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> 类型 指针步长为</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>str1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>[0]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>===</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>str1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>str1[1]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>===</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>(str1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>用数组下标遍历，不会改变原来的指针</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>str1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>的值</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直线箭头连接符 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDF8295F-6AEA-BF42-9CC8-5C036A3AA19A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7035800" y="2374900"/>
+          <a:ext cx="2540000" cy="2717800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="上弧形箭头 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA24B432-19CB-7A44-8F7D-29C73D922B86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="901700" y="3556000"/>
+          <a:ext cx="5067300" cy="1155700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 7924"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="文本框 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067CFF2F-53A5-844F-9C74-689B0B21E0E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9017000" y="4216400"/>
+          <a:ext cx="3111500" cy="2387600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>* 指针和数组名的区别</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>p++:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  这样是可以的。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>str1++:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 这样是不可以的。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 数组名的方向是不可以被改变的</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 数组名是常量数组（方向改变不了）</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>//</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  栈是操作系统开辟和回收的，是根据数组名来找到一块连续内存的首地址，如果首地址变量发生改变。将无法准确回收。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>数组一般在栈上开辟内存。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>指针一般在堆上开辟内存。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文本框 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3883C508-A9BA-7047-A7E4-1D05E05466E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="965200" y="647700"/>
+          <a:ext cx="2209800" cy="2387600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>int</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>main(void)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>buf[20]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>"aaaa";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>buf2[]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>"bbbb";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> *</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>p1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>"111111";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>char</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> *</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>p2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>malloc(100);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>strcpy(p2,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>"3333");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>return</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" baseline="0"/>
+            <a:t>0;</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="左大括号 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F49689-5196-D146-B685-989A1A2BF7AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4483100" y="914400"/>
+          <a:ext cx="279400" cy="1879600"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="左大括号 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBEC163-C4F3-AF46-8B2B-FDAA98607EDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4673600" y="3543300"/>
+          <a:ext cx="215900" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="右大括号 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA6AA0A-B128-8F41-A5D8-1C237435AD69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12052300" y="546100"/>
+          <a:ext cx="165100" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直线箭头连接符 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC09AFF-33D9-0F47-A660-453280153054}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6426200" y="2743200"/>
+          <a:ext cx="762000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直线箭头连接符 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D6C308-1B08-8D42-9477-E8E190D70CBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6426200" y="4368800"/>
+          <a:ext cx="762000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直线箭头连接符 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6144D610-42FF-1146-AB73-45465459BAB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7683500" y="5702300"/>
+          <a:ext cx="2590800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="左大括号 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC555DEF-FFCD-0249-98D0-F1926D5E5433}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4749800" y="5397500"/>
+          <a:ext cx="152400" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="左大括号 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{563F9868-E673-A842-8B79-F96E2C645B1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="6362700"/>
+          <a:ext cx="139700" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直线箭头连接符 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA37D13B-9A47-1E48-ADA5-3161EEEF63E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7569200" y="1231900"/>
+          <a:ext cx="3467100" cy="5791200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1790,7 +4481,7 @@
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1806,31 +4497,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="J1" s="44" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="J1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="2:14" ht="17" thickBot="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="2:14">
@@ -1844,10 +4535,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="47"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="6"/>
       <c r="M3" s="7"/>
       <c r="N3" s="2"/>
@@ -1861,8 +4552,8 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="47"/>
       <c r="L4" s="11"/>
       <c r="M4" s="12"/>
       <c r="N4" s="2"/>
@@ -1876,8 +4567,8 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
       <c r="L5" s="11"/>
       <c r="M5" s="12"/>
       <c r="N5" s="2"/>
@@ -1891,8 +4582,8 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="11"/>
       <c r="M6" s="12"/>
       <c r="N6" s="2"/>
@@ -1906,8 +4597,8 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
       <c r="L7" s="11"/>
       <c r="M7" s="12"/>
       <c r="N7" s="2"/>
@@ -1921,8 +4612,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
       <c r="L8" s="11"/>
       <c r="M8" s="12"/>
       <c r="N8" s="2"/>
@@ -1936,8 +4627,8 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
       <c r="L9" s="11"/>
       <c r="M9" s="12"/>
       <c r="N9" s="2"/>
@@ -1951,8 +4642,8 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
       <c r="L10" s="11"/>
       <c r="M10" s="12"/>
       <c r="N10" s="2"/>
@@ -1966,8 +4657,8 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
       <c r="L11" s="11"/>
       <c r="M11" s="12"/>
       <c r="N11" s="2"/>
@@ -1981,8 +4672,8 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
       <c r="L12" s="11"/>
       <c r="M12" s="12"/>
       <c r="N12" s="2"/>
@@ -1996,8 +4687,8 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
       <c r="L13" s="11"/>
       <c r="M13" s="12"/>
       <c r="N13" s="2"/>
@@ -2011,8 +4702,8 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
       <c r="L14" s="11"/>
       <c r="M14" s="12"/>
       <c r="N14" s="2"/>
@@ -2026,8 +4717,8 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
       <c r="L15" s="11"/>
       <c r="M15" s="12"/>
       <c r="N15" s="2"/>
@@ -2041,8 +4732,8 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
       <c r="L16" s="11"/>
       <c r="M16" s="12"/>
       <c r="N16" s="2"/>
@@ -2056,8 +4747,8 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
       <c r="L17" s="11"/>
       <c r="M17" s="12"/>
       <c r="N17" s="2"/>
@@ -2071,8 +4762,8 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="25"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="2"/>
@@ -2086,8 +4777,8 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
       <c r="L19" s="11"/>
       <c r="M19" s="12"/>
       <c r="N19" s="2"/>
@@ -2101,8 +4792,8 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="25"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
       <c r="L20" s="11"/>
       <c r="M20" s="12"/>
       <c r="N20" s="2"/>
@@ -2116,8 +4807,8 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="25"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
       <c r="L21" s="11"/>
       <c r="M21" s="12"/>
       <c r="N21" s="2"/>
@@ -2131,8 +4822,8 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="25"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
       <c r="L22" s="11"/>
       <c r="M22" s="12"/>
       <c r="N22" s="2"/>
@@ -2148,10 +4839,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="21"/>
+      <c r="K23" s="49"/>
       <c r="L23" s="11"/>
       <c r="M23" s="13"/>
       <c r="N23" s="2"/>
@@ -2167,10 +4858,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="23"/>
+      <c r="K24" s="51"/>
       <c r="L24" s="16"/>
       <c r="M24" s="17"/>
       <c r="N24" s="2"/>
@@ -2227,48 +4918,48 @@
     <row r="28" spans="2:14">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="37"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="38"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="2:14" ht="17" thickBot="1">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="43"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="2:14">
@@ -2319,63 +5010,63 @@
     <row r="34" spans="2:14">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="28"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="26"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="2:14">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="31"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="29"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="2:14">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="31"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="29"/>
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="2:14" ht="17" thickBot="1">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="34"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="32"/>
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="2:14">
@@ -2425,6 +5116,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="D34:M37"/>
     <mergeCell ref="D28:M30"/>
     <mergeCell ref="D1:F2"/>
@@ -2441,16 +5142,6 @@
     <mergeCell ref="J1:M2"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2476,23 +5167,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="38" customHeight="1">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="2:8" ht="26" customHeight="1" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="19"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -2500,8 +5191,8 @@
     <row r="4" spans="2:8">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
       <c r="F4" s="19"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2509,8 +5200,8 @@
     <row r="5" spans="2:8">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="19"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -2518,8 +5209,8 @@
     <row r="6" spans="2:8">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="19"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2529,8 +5220,8 @@
         <v>4</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="19"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2538,8 +5229,8 @@
     <row r="8" spans="2:8">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="19"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2547,8 +5238,8 @@
     <row r="9" spans="2:8">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
       <c r="F9" s="19" t="s">
         <v>13</v>
       </c>
@@ -2558,8 +5249,8 @@
     <row r="10" spans="2:8">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="19"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2567,8 +5258,8 @@
     <row r="11" spans="2:8">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="19"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2576,8 +5267,8 @@
     <row r="12" spans="2:8">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="19"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2585,8 +5276,8 @@
     <row r="13" spans="2:8">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="19"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2594,8 +5285,8 @@
     <row r="14" spans="2:8">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
       <c r="F14" s="19"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2603,8 +5294,8 @@
     <row r="15" spans="2:8">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="19"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -2614,8 +5305,8 @@
         <v>8</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="19"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2623,8 +5314,8 @@
     <row r="17" spans="2:8">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="19"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -2632,8 +5323,8 @@
     <row r="18" spans="2:8">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="19"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2641,8 +5332,8 @@
     <row r="19" spans="2:8">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
       <c r="F19" s="19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2650,8 +5341,8 @@
     <row r="20" spans="2:8">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
       <c r="F20" s="19" t="s">
         <v>14</v>
       </c>
@@ -2661,8 +5352,8 @@
     <row r="21" spans="2:8">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="19"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2670,8 +5361,8 @@
     <row r="22" spans="2:8">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="19"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2679,8 +5370,8 @@
     <row r="23" spans="2:8">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
       <c r="F23" s="19"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2688,8 +5379,8 @@
     <row r="24" spans="2:8">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
       <c r="F24" s="19"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2699,8 +5390,8 @@
         <v>4</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="19"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2708,8 +5399,8 @@
     <row r="26" spans="2:8">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
       <c r="F26" s="19" t="s">
         <v>16</v>
       </c>
@@ -2719,8 +5410,8 @@
     <row r="27" spans="2:8">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="19"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2728,8 +5419,8 @@
     <row r="28" spans="2:8" ht="17" thickBot="1">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="51"/>
       <c r="F28" s="19"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -2754,15 +5445,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
@@ -2775,12 +5463,15 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,125 +5484,844 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E04129F-37F1-5E4C-BBF3-A1A8900FBE60}">
   <dimension ref="E3:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="51" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="51"/>
-    <col min="5" max="5" width="14.83203125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="21" style="51" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="51" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="51" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="51"/>
+    <col min="1" max="1" width="14.83203125" style="20" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="20"/>
+    <col min="5" max="5" width="14.83203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="21" style="20" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="3" spans="5:8">
-      <c r="E3" s="51" t="s">
+      <c r="F3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8">
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="5:8">
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="5:8">
+      <c r="F6" s="22">
+        <v>10</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="5:8">
-      <c r="F4" s="52"/>
-    </row>
-    <row r="5" spans="5:8">
-      <c r="F5" s="53"/>
-    </row>
-    <row r="6" spans="5:8">
-      <c r="F6" s="53">
-        <v>10</v>
-      </c>
-      <c r="H6" s="51" t="s">
+    </row>
+    <row r="7" spans="5:8">
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="5:8">
+      <c r="E8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="5:8">
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="5:8">
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="5:8">
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="5:8">
+      <c r="F12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="5:8">
-      <c r="F7" s="53"/>
-    </row>
-    <row r="8" spans="5:8">
-      <c r="E8" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="53"/>
-    </row>
-    <row r="9" spans="5:8">
-      <c r="F9" s="52"/>
-    </row>
-    <row r="10" spans="5:8">
-      <c r="F10" s="52"/>
-    </row>
-    <row r="11" spans="5:8">
-      <c r="F11" s="54"/>
-    </row>
-    <row r="12" spans="5:8">
-      <c r="F12" s="54" t="s">
+    <row r="13" spans="5:8">
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="5:8">
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="5:8">
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="5:8">
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="5:8">
+      <c r="F18" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H18" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="5:8">
-      <c r="F13" s="54"/>
-    </row>
-    <row r="14" spans="5:8">
-      <c r="F14" s="54"/>
-    </row>
-    <row r="15" spans="5:8">
-      <c r="F15" s="52"/>
-    </row>
-    <row r="16" spans="5:8">
-      <c r="F16" s="52"/>
-    </row>
-    <row r="17" spans="5:8">
-      <c r="F17" s="53"/>
-    </row>
-    <row r="18" spans="5:8">
-      <c r="F18" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="51" t="s">
+    <row r="19" spans="5:8">
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="5:8">
+      <c r="E20" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="5:8">
-      <c r="F19" s="53"/>
-    </row>
-    <row r="20" spans="5:8">
-      <c r="E20" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="53"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="5:8">
-      <c r="F21" s="52"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="5:8">
-      <c r="F22" s="52"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="5:8">
-      <c r="F23" s="52"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="24" spans="5:8">
-      <c r="F24" s="52"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="5:8">
-      <c r="F25" s="52"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="26" spans="5:8">
-      <c r="F26" s="52"/>
+      <c r="F26" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CB3B8B-DBB5-CC4E-80CA-40A5C6081C04}">
+  <dimension ref="E3:N36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="5" width="10.83203125" style="20"/>
+    <col min="6" max="6" width="23.5" style="57" customWidth="1"/>
+    <col min="7" max="7" width="21.5" style="20" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:14">
+      <c r="F3" s="56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="5:14">
+      <c r="K4" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="5:14">
+      <c r="F5" s="56"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+    </row>
+    <row r="6" spans="5:14">
+      <c r="F6" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="62"/>
+    </row>
+    <row r="7" spans="5:14">
+      <c r="F7" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="5:14">
+      <c r="E8" s="20">
+        <v>5</v>
+      </c>
+      <c r="F8" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="5:14">
+      <c r="F9" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="5:14">
+      <c r="F10" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="66"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="5:14">
+      <c r="F11" s="56"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="12" spans="5:14">
+      <c r="F12" s="56"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="5:14">
+      <c r="F13" s="56"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+    </row>
+    <row r="14" spans="5:14">
+      <c r="F14" s="58"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
+    </row>
+    <row r="15" spans="5:14">
+      <c r="F15" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+    </row>
+    <row r="16" spans="5:14">
+      <c r="F16" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+    </row>
+    <row r="17" spans="5:14">
+      <c r="E17" s="20">
+        <v>128</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+    </row>
+    <row r="18" spans="5:14">
+      <c r="F18" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+    </row>
+    <row r="19" spans="5:14">
+      <c r="F19" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+    </row>
+    <row r="20" spans="5:14">
+      <c r="F20" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+    </row>
+    <row r="21" spans="5:14">
+      <c r="F21" s="56"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+    </row>
+    <row r="22" spans="5:14">
+      <c r="F22" s="56"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+    </row>
+    <row r="23" spans="5:14">
+      <c r="F23" s="56"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+    </row>
+    <row r="24" spans="5:14">
+      <c r="F24" s="61"/>
+      <c r="G24" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+    </row>
+    <row r="25" spans="5:14">
+      <c r="E25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="61"/>
+      <c r="G25" s="63"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+    </row>
+    <row r="26" spans="5:14">
+      <c r="F26" s="61"/>
+      <c r="G26" s="63"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+    </row>
+    <row r="27" spans="5:14">
+      <c r="F27" s="61"/>
+      <c r="G27" s="63"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+    </row>
+    <row r="28" spans="5:14">
+      <c r="F28" s="56"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+    </row>
+    <row r="29" spans="5:14">
+      <c r="F29" s="56"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+    </row>
+    <row r="30" spans="5:14">
+      <c r="F30" s="61"/>
+      <c r="G30" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+    </row>
+    <row r="31" spans="5:14">
+      <c r="F31" s="61"/>
+      <c r="G31" s="63"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+    </row>
+    <row r="32" spans="5:14">
+      <c r="F32" s="61"/>
+      <c r="G32" s="63"/>
+    </row>
+    <row r="33" spans="6:7">
+      <c r="F33" s="61"/>
+      <c r="G33" s="63"/>
+    </row>
+    <row r="34" spans="6:7">
+      <c r="F34" s="56"/>
+    </row>
+    <row r="35" spans="6:7">
+      <c r="F35" s="56"/>
+    </row>
+    <row r="36" spans="6:7">
+      <c r="F36" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="G24:G27"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF02F1A5-579B-6C4B-AE4C-80CB088C4869}">
+  <dimension ref="C1:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="20"/>
+    <col min="7" max="7" width="27.33203125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="20"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15">
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="3:15">
+      <c r="G2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+    </row>
+    <row r="3" spans="3:15">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+    </row>
+    <row r="4" spans="3:15">
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+    </row>
+    <row r="5" spans="3:15">
+      <c r="G5" s="22"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+    </row>
+    <row r="6" spans="3:15">
+      <c r="G6" s="22"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+    </row>
+    <row r="7" spans="3:15">
+      <c r="G7" s="22"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="55">
+        <v>100</v>
+      </c>
+      <c r="O7" s="55"/>
+    </row>
+    <row r="8" spans="3:15">
+      <c r="G8" s="22"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+    </row>
+    <row r="9" spans="3:15">
+      <c r="F9" s="20">
+        <v>20</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+    </row>
+    <row r="10" spans="3:15">
+      <c r="G10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+    </row>
+    <row r="11" spans="3:15">
+      <c r="G11" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="55"/>
+      <c r="L11" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="73"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+    </row>
+    <row r="12" spans="3:15">
+      <c r="G12" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+    </row>
+    <row r="13" spans="3:15">
+      <c r="G13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+    </row>
+    <row r="14" spans="3:15">
+      <c r="G14" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+    </row>
+    <row r="18" spans="6:15">
+      <c r="G18" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15">
+      <c r="G19" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15">
+      <c r="F20" s="20">
+        <v>5</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15">
+      <c r="G21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15">
+      <c r="G22" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="6:15">
+      <c r="K23" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="70"/>
+      <c r="O23" s="70"/>
+    </row>
+    <row r="24" spans="6:15">
+      <c r="K24" s="68"/>
+      <c r="L24" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
+    </row>
+    <row r="25" spans="6:15">
+      <c r="K25" s="68"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+    </row>
+    <row r="26" spans="6:15">
+      <c r="K26" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" s="72"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
+    </row>
+    <row r="27" spans="6:15">
+      <c r="G27" s="23"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+    </row>
+    <row r="28" spans="6:15">
+      <c r="G28" s="23"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+    </row>
+    <row r="29" spans="6:15">
+      <c r="F29" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="23"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
+    </row>
+    <row r="30" spans="6:15">
+      <c r="G30" s="23"/>
+      <c r="H30" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="72"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="62"/>
+    </row>
+    <row r="31" spans="6:15">
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+    </row>
+    <row r="32" spans="6:15">
+      <c r="G32" s="23"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+    </row>
+    <row r="33" spans="6:15">
+      <c r="F33" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="23"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+    </row>
+    <row r="34" spans="6:15">
+      <c r="G34" s="23"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="62"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="62"/>
+    </row>
+    <row r="35" spans="6:15">
+      <c r="G35" s="23"/>
+      <c r="H35" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+    </row>
+    <row r="36" spans="6:15">
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="M6:M8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F003B54-18DF-4441-81E9-8E67CC05B6EF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] c language review , reverse string array use recursion
</commit_message>
<xml_diff>
--- a/C内存图.xlsx
+++ b/C内存图.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yytd/luochao/github_lc/c_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E40A681-27D7-5B46-A572-E1EA8ED42F4C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E672876-9767-574B-98DD-0F1F85B08603}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="1880" windowWidth="25200" windowHeight="16760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18200" yWindow="3680" windowWidth="25200" windowHeight="16760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据类型的本质" sheetId="1" r:id="rId1"/>
     <sheet name="虚拟内存" sheetId="2" r:id="rId2"/>
     <sheet name="指针" sheetId="3" r:id="rId3"/>
     <sheet name="变量的本质" sheetId="4" r:id="rId4"/>
-    <sheet name="str++和p++、sizeof" sheetId="5" r:id="rId5"/>
-    <sheet name="字符串的内存四区图" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
+    <sheet name="代码内存四区图" sheetId="7" r:id="rId5"/>
+    <sheet name="str++和p++、sizeof" sheetId="5" r:id="rId6"/>
+    <sheet name="字符串的内存四区图" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>1G（物理内存）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,6 +416,62 @@
   </si>
   <si>
     <t>0x10000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main(){   }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demo() {}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123456'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出栈销毁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -641,7 +697,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -810,6 +866,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,6 +902,9 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,6 +925,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1767,6 +1844,576 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>850900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直线连接符 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9813503B-AEA6-4E4C-915A-3972E93A4966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3276600" y="1612900"/>
+          <a:ext cx="3911600" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直线箭头连接符 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B340DE41-12C2-8743-AB41-271AE5CEED31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7175500" y="2387600"/>
+          <a:ext cx="2400300" cy="1384300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="左大括号 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{915CD902-313B-1C40-AC3B-7C0A7B5D2718}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9461500" y="622300"/>
+          <a:ext cx="342900" cy="1739900"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>174700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>147774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685802</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="下弧形箭头 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FCE4232-77E8-484D-B07A-FA0DC480A4D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3977588" y="2351986"/>
+          <a:ext cx="2481125" cy="511102"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="直线箭头连接符 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CE418DB-1E8E-E940-A475-F4E983836A7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7353300" y="1524000"/>
+          <a:ext cx="1943100" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>513</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="图片 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB15C204-B274-EC45-908F-5F6B063CFEF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="660400"/>
+          <a:ext cx="4178813" cy="6299200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直线连接符 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D726FCF2-C36A-6541-92DF-DF0B119BBB60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5080000" y="2832100"/>
+          <a:ext cx="4356100" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直线箭头连接符 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE38A99-B40C-C44D-8E52-91EDFEF2E65B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11963400" y="2413000"/>
+          <a:ext cx="482600" cy="2590800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>135760</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>118760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>252440</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160320</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="35" name="墨迹 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6EC262-8787-E94F-B2D3-5B000DDC0884}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4428360" y="1541160"/>
+            <a:ext cx="11495880" cy="5324760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="35" name="墨迹 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6EC262-8787-E94F-B2D3-5B000DDC0884}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4419720" y="1532520"/>
+              <a:ext cx="11513520" cy="5342400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>661480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>661840</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101440</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="36" name="墨迹 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E78CE982-5528-A446-9A96-B4EEC48ACEDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13031280" y="1117080"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="36" name="墨迹 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E78CE982-5528-A446-9A96-B4EEC48ACEDF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13022280" y="1108080"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -3378,7 +4025,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4164,6 +4811,65 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-02-27T07:32:28.767"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">8571 13 24575,'11'0'0,"1"0"0,-1 0 0,0 0 0,0 0 0,5 0 0,-3 0 0,28 0 0,-24 0 0,44 5 0,-44-4 0,39 4 0,-40-5 0,30 5 0,-36-9 0,34 13 0,-32-13 0,43 9 0,-37-5 0,33 0 0,-36 0 0,21 0 0,-23 0 0,8 0 0,-10 0 0,1 0 0,-1 0 0,45 5 0,-26-4 0,21 2 0,-1-1 0,-21-2 0,45 0 0,-58 0 0,15 0 0,-20 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,5 0 0,-4 0 0,49 0 0,-39 0 0,64 0 0,-67 0 0,46 0 0,-47 0 0,28 0 0,-33 0 0,8 0 0,-9 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,25 0 0,-19 0 0,49 0 0,-48 0 0,53 0 0,-52 0 0,22 0 0,-30 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,5-5 0,-4 4 0,4-4 0,-5 5 0,1 0 0,-1 0 0,0 0 0,0 0 0,25 0 0,-19 0 0,29-5 0,-32 3 0,17-3 0,-17 5 0,17-5 0,-18 4 0,8-4 0,-9 5 0,-1 0 0,-5-5 0,4 4 0,-4-4 0,5 5 0,-5 5 0,-1-9 0,0 8 0,2-9 0,4 5 0,0 0 0,0 0 0,-5 5 0,-1-4 0,-5 4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="584989">20920 321 24575,'0'11'0,"5"15"0,-4-11 0,4 21 0,-5-18 0,10 34 0,-8-28 0,18 61 0,-17-62 0,7 47 0,-10-55 0,5 21 0,-4 8 0,4-1 0,-5 17 0,0-31 0,0 22 0,5-14 0,-4 4 0,4-5 0,-5-23 0,0 3 0,0-5 0,5 15 0,-4-6 0,4 7 0,-5-11 0,0 0 0,0-3 0,0 13 0,5-12 0,-4 36 0,4-31 0,-5 32 0,0-37 0,0 12 0,0-14 0,0 4 0,0-5 0,0 0 0,5 15 0,-4-11 0,9 61 0,-8-52 0,-2 56 0,-2-64 0,-3 15 0,5-20 0,0 1 0,-5 14 0,4-11 0,-9 35 0,9-32 0,-4 18 0,0-30 0,3 4 0,-8 16 0,4-10-6784,-10 65 6784,8-58 0,-3 28 0,2-1 0,7-29 0,-13 25 0,13-36 0,-3-4 0,5 5 0,0 0 6784,0 0-6784,0 0 0,-5-4 0,4 3 0,-4-4 0,5 5 0,0 0 0,0 15 0,0-11 0,0 16 0,0-19 0,0 5 0,0-6 0,0 0 0,0-5 0,0-1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="776280">1469 1568 24575,'11'-5'0,"0"4"0,1-4 0,-1 0 0,0-1 0,0-1-4252,46-8 1,10-1 4251,-20 3 704,10-1 1,11 0-705,23 2 0,-6 5-1664,-14 4 1664,-5-2 0,19-1 0,1 0 0,-19 2 0,15 2 0,-11 0 0,28 0 0,14-2 0,3 1 0,-12 1 0,-23 0-1024,-9 0 1,3 2 1023,-12 0 0,19 1 0,14-1 0,9 2 0,5-1 0,1 1 0,-6 0 0,-8 0 0,-15 0 0,-18 1 0,13 3 0,0 1 0,-10-2 0,19 1 0,12 0 0,10 0 0,4 1 0,0-1 0,-4 1 0,-9-1 0,-12 0 0,23 1 0,-14 0 0,-2 0 0,5 1 0,-4-2 0,3 1 0,2 1 0,0-2 0,0-1 0,-11-1 0,6 0 0,0-1 0,-5-1 0,-12 0 0,-17-3 0,31-5 0,-10 0 0,23-1 0,-2-1 0,-28-1 4792,-15-4-4792,39-13 0,-7 3 0,-61 18 334,28-22-334,-48 26 2102,0-9-2102,-5 4 0,29-16 0,-23 13-1604,65-8 1,14 3 1603,-27 10 0,8-4 0,24-3 0,3 0 0,-20 3-2269,-21 5 1,-3 0 2268,12-3 0,8-2 0,8 0-607,-6 2 0,10-1 0,2 0 1,-7 1-1,-14 1 607,-7 1 0,5 1-226,-3-1 1,20 0-1,15-1 1,8-1 0,4 1-1,-3 0 1,-8 0 0,-13 1-1,-19 2 226,12 0 0,1 2 0,-17-2 0,19 1 0,13-1 0,9 0 0,4 0 0,0 0 0,-4 0 0,-10 0 0,-13 1 0,-19 0 0,13 0 0,-3 0 0,5 0 0,23 0 0,13 1 0,4-1 0,-7 1 0,-17 1 0,-27 1 0,16 6 0,-5-5 0,24-1 0,-3-1 0,-29 2 0,-22 4 1014,27-7 1,-7 0-1015,-51 0 3034,15 0-3034,-20 0 4537,5 0-4537,-3 0 0,39 2 0,7 1 0,-17-2-2269,58 5 1,-1 3 2268,-58-2-1012,32 2 1,23 2 0,-20-1 1011,-21 0-677,34 1 1,26 2 0,-25-3 676,-29-7 0,4 4 0,22 2 0,0 0 0,-23-3 0,-6-1 0,25 1 0,22 3 0,-27-3 0,-42-5 0,50 4 0,-3 0 0,-58-4 2029,44 4-2029,-63 0 3034,4-4-3034,-9 9 0,29 1 0,-24 2 0,58 18 0,-49-16 0,45 15 0,4-2 0,-33-13 0,54 31 0,1 0 0,-55-33-1012,25 17 1,18 10 0,-15-12 1011,-16-17-677,18 16 1,17 9 0,-16-9 676,-20-15 73,42 23 0,-4 2-73,-54-26 500,30 7 1,-4 2-501,-36-8 2314,51 14-2314,-56-12 0,73 37 0,-60-33-30,47 23 1,2 1 29,-42-20-716,54 28 1,2-2 715,-48-31-620,21 14 1,17 11 0,-16-10 619,-17-13 0,13 10 0,13 9 0,-18-8 0,-25-10-57,50 24 1,0 2 56,-52-24 0,52 35 0,-2 2 0,-53-33 0,44 36 0,2-1 0,-42-38 0,36 39 0,-1-1 0,-37-39 159,26 43 0,-1 0-159,-29-45 0,31 50 0,3 3 0,-28-44 0,24 36 0,18 22 0,-15-19 2162,-17-23-2162,14 30 0,11 22 0,-15-23 3257,-24-38-3257,17 42 0,-4-4 0,-23-53-354,16 36 0,-2 2 354,-18-32 392,16 46 0,1 0-392,-15-45-1629,16 60 1,2 3 1628,-9-48 0,3 37 0,3 26 0,-4-22-485,-1-26 485,-5 11 0,5 30 0,1 11 0,-1-8 0,-5-26 0,4 14 0,-8-23 0,5 23 0,0 12 0,1 0 0,-4-12 0,-4-23 0,-2 25 0,0-7 0,3 27 0,0-2 0,-4-29 0,-5-13 0,1 5 0,0 24 0,-1-1 0,0-27 0,-1-15 0,3 14 0,3 25 0,0-1 0,-2-26 0,1-20 0,0 20 0,1 26 0,-1 0 0,-2-25 0,-3-14 0,-1 18 0,0 26 0,-1 1 0,1-29 0,0-18 0,-1 31 0,-1 12 0,-2-17 0,-2 3-163,0-2 0,0 7 1,-1-3 162,3-16 0,0-1 0,-1 7 0,-1 6 0,-2 15 0,0 1 0,1-10 0,0-21 0,-4 9-396,3 5 0,-1 25 1,-1-1-1,2-28 396,-2-22 0,-3 27 0,-4 22 0,5-23 0,5-29 0,-6 13 0,-5 15 0,3-17 0,6-24 0,-10 45 0,-4-1 0,0-47 0,-4 52 0,-1 1 0,2-45 0,-3 14 0,-9 21 0,-1 2 0,6-17 0,-12 10 0,4-13 0,-16 22 0,-10 10 0,-1 1 0,7-10 0,15-20 0,10-13 0,-3 0 0,-10 6 0,-17 17 0,-11 10 0,-4 2 0,4-3 0,10-11 0,18-18 0,11-10 0,-1-2 0,-19 13 0,-21 16 0,-11 9 0,0-1 0,10-9 0,21-18 0,20-16 0,0-2 0,-23 15 0,-19 15 0,-8 4 0,9-8 0,20-18 0,-2-9 0,3 4 0,-17 14 0,1-2 0,18-15 0,4-13 0,-21 21 0,-18 16 0,18-11 0,18-13 0,-23 13 0,-21 11 0,20-10 0,22-8 0,-4-6 0,-23 6 0,0 0 0,18-9 0,-9 1 838,-8 1 0,-14 2-838,12-12 0,-6-1 0,17-5 0,-7-2 0,23-2 0,-17 5 0,-12 2 0,-5 0 0,3-1 0,8-3 0,-10-2 0,4-3 0,2-1 0,-1 2 0,2 3 0,3 1 0,-4 0 0,-11-2 0,16-4 0,-13-1 0,-7-1 0,-3 0 0,2-1 0,8 0 0,10-1 0,17 0 574,-10-1 0,-2 0-574,8 1 0,-20 1 0,-16 1 0,-8 1 0,-3 0 0,2 0 0,10-1 0,15 0 0,21-1 0,-7 0 0,0 0 0,10 1 0,-19 2 0,-14 0 0,-9 1 0,-2 0 0,3 0 0,8-1 0,14-1 0,20-1 0,-6-1 0,1 0 0,7 0 0,-19 0 0,-13 1 0,-9 0 0,-2 1 0,2-1 0,8 0 0,13-1 0,18-1 0,-14-1 0,0 0 0,14-1 0,-19 1 0,-14 0 0,-7 0 0,-3 0 0,3 0 0,7 0 0,14 0 0,18-1 0,-13 1 0,0-2 0,14 1 0,-19 0 0,-13-1 0,-8 1 0,-3-1 0,3 0 0,9 0 0,13 0 0,19-1 0,-8-3 0,0 0 0,2 2 0,-20 0 0,-15 0 0,-7 0 0,1 0 0,6-1 0,14 1 0,22 0 0,-4-3 0,3 0 0,-5 2 0,-20 0 0,-11 0 0,2 0 0,12 1 0,23 1 0,17 1 0,2 0 0,-30-3 0,-20-1 0,0-1 0,25 2 0,0 1 0,-6-4 0,-27-4 0,0 0 0,27 3 0,4 2 0,8-1 0,-25-3 0,-10 0 0,10 0 0,26 4 0,-3 1 0,-4-1 0,-26-3 0,3 0 0,30 4 0,29 2 0,-36-6 0,-23-4 0,24 1 0,35 1 0,-43-11 0,-29-7 0,24 5 0,31 6 0,-18-5 0,-30-9 0,-1-1 0,26 8 0,4 3 0,-3-3 0,-28-9 0,2 0 0,28 7 0,12 1 0,-3-2 0,-22-8 0,1-1 0,24 10 0,11 3 0,-10-11 0,-22-14 0,1-1 0,24 13 0,14 6 0,-7-10 0,-19-18 0,0 0 0,20 15 0,9 8 0,-17-30 0,-16-20 0,15 20 0,14 24 0,10-9 0,-9-20 0,1-1 0,12 17 0,4 3 0,0-8 0,-9-22 0,0-2 0,12 21 0,5-1 0,-1-8 0,-8-26 0,0-1 0,8 25 0,0 2 0,4-6 0,-5-26 0,0 0 0,6 28 0,2 15 0,2-10 0,-4-24 0,1-1 0,4 26 0,2 13 0,3-15 0,0-27 0,0-2 0,2 23 0,-2-5 0,3 2 0,-1-26 0,0-1 0,3 24 0,0-8 0,1 22 0,-2-21 0,0-7 0,0 6 0,3 21 0,1 20 0,0-2 0,-1-17 0,-2-23 0,0-12 0,0 0 0,0 10 0,2 23 0,-1 11 0,2-1 0,0-5 0,1-22 0,-1-12 0,1-4 0,0 4 0,1 12 0,1 21 0,3 4 0,0 2 0,0-7 0,1-20 0,1-10 0,-1 2 0,1 12 0,-2 22 0,6-22 0,-1 4 0,4-24 0,-1 0 0,-4 25 0,-3-1 0,6 0 0,5-25 0,0-1 0,-5 26 0,-4-2 0,4 0 0,5-28 0,0 2 0,-3 27 0,-1 8 0,0-6 0,3-27 0,1 0 0,-5 28 0,2 10 0,-2 5 0,5-23 0,1-8 0,-2 7 0,-5 24 0,1-9 0,2 7 0,6-23 0,3-8 0,-2 9 0,-7 26 0,-2 7 0,6-20 0,7-29 0,1-1 0,-7 28 0,-2 15 0,3-25 0,5-24 0,-1 24 0,4 25 0,-13 7 0,0-5-1005,8 3 1,-3 9 1004,-13 18 811,10-24 0,8-17 0,-2 6-811,-6 12 0,0 3 907,4-15 1,2-1-908,-1 6 0,-5 13 0,-13 28 0,31-67 0,-30 63 0,17-28 0,0 0 0,-16 29-1220,34-60 1220,-36 65-2630,42-63 2630,-38 58 0,25-37 0,1-1 0,-25 32 1315,18-27 0,2 5-1315,-19 37 1220,11-25-1220,-16 32 4537,0-1-4537,-4-3 6784,4 4-6784,0-5 0,21-41 0,-15 31 0,39-61 0,-44 64 0,24-24 0,-29 31 0,4 0 0,-5-1 0,0 1 0,5 5 0,-4-4 0,4 3 0,5-29 0,-8 13 0,8-14 0,-10 20 0,5 11 0,-3-9 0,2 2 0,1-4 0,7-30 0,-5 29 0,8-39 0,-14 42 0,4-11 0,0 19 0,-9 2 0,8 5 0,-9 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="778811">17665 11367 24575,'11'0'0,"0"0"0,0 0 0,28 0 0,9 0 0,-2 5-1418,14 5 1,30 6 0,16 3 0,3 2 0,-7-1 0,-23-4 1417,2 3 0,7 1 0,-24-7 0,19 4 0,13 1 0,11 2 0,6 2 0,2-1 0,-2 0 0,-5 0 0,-9-3 0,-14-1 0,-17-4-401,7 2 0,-18-3 0,17 3 401,-9-1 0,16 3 0,12 2 0,9 2 0,4 2 0,2-1 0,-3 1 0,-5-2 0,-9-1 0,-12-3 0,-17-2 0,25 6 0,-3 2 0,-16-4 0,16 5 0,14 4 0,6 2 0,3 1 0,-3-1 0,-8-2 0,-13-3 0,-18-6 0,11 4 0,-5 1 0,-1 3 0,17 8 0,8 4 0,-2 0 0,-13-5 0,-22-9-386,9 8 386,3 9 0,-19-2 0,-51-29-1721,-2 38 1,-1 8 1720,-5-15 1720,7 10 1,-5 4-1721,-33 27 2816,25-48-2816,-44 39 0,-6 0 0,31-38 0,-41 12 0,-27 9 0,20-13-104,21-14 104,-12-4 0,-27 7 0,-8-2 0,13-9 0,14-13 0,7-6 0,-3 1 0,-6 8 0,-3 2 0,-3-9 0,1-14 0,-8-10 0,8-3 0,20 5-86,-1-6 86,9-8 0,-17-14 0,2 1 0,22 10 0,17 7 0,-27-40 0,9 1 592,47 44-592,-8-28 0,3-1 0,11 27 0,8-28 0,4-1 0,-1 24 0,17-20 0,3 1 0,-10 19 0,24-19 0,3 5 0,-17 26-2224,46-28 1,4 2 2223,-30 32-1012,20-9 1,19-7 0,-17 9 1011,-15 12-406,5 3 0,25 0 1,10 0-1,-6 2 0,-21 2 406,-19 4 0,2 1 0,19 1 0,26 0 0,13 1 0,0 1 0,-13-1 0,-25-1 0,-20-1 0,-1 3 0,11 0 0,22 5 0,12 1 0,4 1 0,-4 0 0,-13-2 0,-22-4 0,-12-3 0,0 2 0,13 5 0,22 7 0,12 4 0,5 2 0,-4-1 0,-13-4 0,-21-5 0,-11-2 0,0 0 0,14 6 0,20 7 0,11 4 0,0 0 0,-12-3 0,-21-7 0,-16-5 0,-1 0 0,22 7 0,22 7 0,6 3 0,-8-3 0,-23-7 0,12 6 0,-5-2 0,23 9 0,-3 1 0,-31-9 0,-27-4 782,42 16 1,-13-3-783,-61-24 0,20 32 0,-24-29 0,4 49 0,-5-48 0,-20 78 0,15-71 0,-20 42 0,-1 4 0,18-34 0,-21 21 0,-12 18 0,7-14 0,10-8-522,-30 17 1,-21 17-1,16-20 522,19-24 0,-25 6 0,-20 7 0,19-17 0,31-26 0,-57 9 0,0-8 0,57-20 0,-34-10 0,2-3 0,39 5 0,-25-27 0,4-3 0,32 25 233,-21-43 0,3-4-233,23 37 0,-1-45 0,5 1 0,9 44 360,13-36 0,3 1-360,-6 39 0,24-32 0,0 0 0,-24 33 0,50-37 0,8 1 0,-35 32 0,42-11 0,29-9 0,-17 13 1149,-8 13-1149,-13 11 0,25-2 0,13-1 0,1 1 0,-9 3 0,-22 3 914,-9 3 1,3 4-915,-2 2 0,20 2 0,13 2 0,8 1 0,-1 0 0,-6 1 0,-14-1 0,-20-1 0,2 3 0,-1 3 0,-1 0 0,21 5 0,12 3 0,7 1 0,0 1 0,-7-1 0,-14-3 0,-21-3 355,-3 1 0,0 3-355,3-1 0,21 7 0,13 5 0,8 2 0,0 0 0,-7-2 0,-14-4 0,-21-5 0,-2 0 0,0 2 0,1 1 0,20 9 0,14 4 0,6 4 0,-1-1 0,-6-2 0,-14-5 0,-19-8 0,-4-1 0,-2 1 0,21 9 0,24 13 0,5 2 0,-12-5 0,-31-13 4442,-18-5-4442,22 10 0,-18-5 1381,-51-26-1381,-1 4 0,-19-4 0,16 6 2428,-16-1-2428,-22 25 0,22-19 0,-46 29 0,50-37 0,-31 5 0,32-14 3259,-11 0-3259,14 0 0,1 0 0,5-5 0,-4 4 0,8-9 0,-8 4 0,-36-19 0,-7-3 0,13 6 0,-15-6 0,-23-12 0,-1-1 0,20 10 0,1-3 0,2 3 0,-22-12 0,-7-4 0,8 4 0,21 12 0,1 0 0,-19-11 0,-16-11 0,29 15 0,45 26 0,-37-56 0,51 49 0,-8-78 0,18 53-3392,-5-14 0,0 0 3392,6 17-2424,16-50 2424,-15 70 0,26-45 0,-22 50 0,32-61 0,-29 54-1867,16-25 0,0 0 1867,-20 26-1249,34-22 1,3 2 1248,-29 27 0,60-20 0,7 2 0,-44 19-237,21 6 1,28 0 0,1 1 0,-22 1 236,0 0 0,-11 7 0,24 4 0,17 2 0,6 1 0,-4 1 0,-12-1 0,-22-1 0,-7 2 0,3 2 0,-2-4 0,21 2 0,14 2 0,10 0 0,2 0 0,-2 1 0,-8-2 0,-14-1 0,-20-2 0,9 2 0,-1 0 0,-7-2 0,20 2 0,13 1 0,5 0 0,0 1 0,-9-2 0,-14-1 0,-21-2 0,36 1 0,-27 0 0,23 3 0,5 1 0,-11-2 0,-28-4 0,-19-2 0,30 3 0,-14-1 0,-52-5 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-02-27T07:46:43.015"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5605,6 +6311,418 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F003B54-18DF-4441-81E9-8E67CC05B6EF}">
+  <dimension ref="B2:O34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="56" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15">
+      <c r="G2" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" s="20"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" s="20"/>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" s="20"/>
+      <c r="G6" s="23"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" s="20"/>
+      <c r="G7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="B8" s="20"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="68">
+        <v>100</v>
+      </c>
+      <c r="J8" s="68"/>
+      <c r="K8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="20"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" s="20"/>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="B14" s="20"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="68"/>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="20"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="20"/>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="20"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="20"/>
+      <c r="G19" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="20"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="20"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="20"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="20"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="79" t="s">
+        <v>76</v>
+      </c>
+      <c r="L23" s="77"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="76"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="20"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="76"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="20"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="76"/>
+      <c r="O25" s="76"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="20"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="20"/>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="76"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="76"/>
+      <c r="O27" s="76"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="20"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="20"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="76"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="20"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="76"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="20"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="76"/>
+      <c r="N31" s="76"/>
+      <c r="O31" s="76"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="I32" s="76"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="76"/>
+      <c r="O32" s="76"/>
+    </row>
+    <row r="33" spans="9:15">
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="76"/>
+      <c r="O33" s="76"/>
+    </row>
+    <row r="34" spans="9:15">
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K23:K28"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CB3B8B-DBB5-CC4E-80CA-40A5C6081C04}">
   <dimension ref="E3:N36"/>
   <sheetViews>
@@ -5615,13 +6733,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="5" width="10.83203125" style="20"/>
-    <col min="6" max="6" width="23.5" style="57" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="58" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="20" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="3" spans="5:14">
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5631,39 +6749,39 @@
       </c>
     </row>
     <row r="5" spans="5:14">
-      <c r="F5" s="56"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
+      <c r="F5" s="57"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
     </row>
     <row r="6" spans="5:14">
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62" t="s">
+      <c r="I6" s="63"/>
+      <c r="J6" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62" t="s">
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="62"/>
+      <c r="N6" s="63"/>
     </row>
     <row r="7" spans="5:14">
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="61" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
@@ -5672,282 +6790,282 @@
       <c r="E8" s="20">
         <v>5</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="5:14">
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="61" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
     </row>
     <row r="10" spans="5:14">
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="61" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65" t="s">
+      <c r="I10" s="66"/>
+      <c r="J10" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="66"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
     </row>
     <row r="11" spans="5:14">
-      <c r="F11" s="56"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
+      <c r="F11" s="57"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
     </row>
     <row r="12" spans="5:14">
-      <c r="F12" s="56"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
+      <c r="F12" s="57"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
     </row>
     <row r="13" spans="5:14">
-      <c r="F13" s="56"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
+      <c r="F13" s="57"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="5:14">
-      <c r="F14" s="58"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
+      <c r="F14" s="59"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
     </row>
     <row r="15" spans="5:14">
-      <c r="F15" s="58" t="s">
+      <c r="F15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
     </row>
     <row r="16" spans="5:14">
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
     </row>
     <row r="17" spans="5:14">
       <c r="E17" s="20">
         <v>128</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="65"/>
     </row>
     <row r="18" spans="5:14">
-      <c r="F18" s="59" t="s">
+      <c r="F18" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="64"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="65"/>
     </row>
     <row r="19" spans="5:14">
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="64"/>
-      <c r="N19" s="64"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="N19" s="65"/>
     </row>
     <row r="20" spans="5:14">
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="60" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
     </row>
     <row r="21" spans="5:14">
-      <c r="F21" s="56"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
+      <c r="F21" s="57"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
     </row>
     <row r="22" spans="5:14">
-      <c r="F22" s="56"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
+      <c r="F22" s="57"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
     </row>
     <row r="23" spans="5:14">
-      <c r="F23" s="56"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
+      <c r="F23" s="57"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
     </row>
     <row r="24" spans="5:14">
-      <c r="F24" s="61"/>
-      <c r="G24" s="63" t="s">
+      <c r="F24" s="62"/>
+      <c r="G24" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
     </row>
     <row r="25" spans="5:14">
       <c r="E25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="63"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="64"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
     </row>
     <row r="26" spans="5:14">
-      <c r="F26" s="61"/>
-      <c r="G26" s="63"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="64"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
     </row>
     <row r="27" spans="5:14">
-      <c r="F27" s="61"/>
-      <c r="G27" s="63"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="64"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
     </row>
     <row r="28" spans="5:14">
-      <c r="F28" s="56"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
+      <c r="F28" s="57"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="65"/>
     </row>
     <row r="29" spans="5:14">
-      <c r="F29" s="56"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
+      <c r="F29" s="57"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="65"/>
     </row>
     <row r="30" spans="5:14">
-      <c r="F30" s="61"/>
-      <c r="G30" s="63" t="s">
+      <c r="F30" s="62"/>
+      <c r="G30" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
     </row>
     <row r="31" spans="5:14">
-      <c r="F31" s="61"/>
-      <c r="G31" s="63"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="64"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
     </row>
     <row r="32" spans="5:14">
-      <c r="F32" s="61"/>
-      <c r="G32" s="63"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="64"/>
     </row>
     <row r="33" spans="6:7">
-      <c r="F33" s="61"/>
-      <c r="G33" s="63"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="64"/>
     </row>
     <row r="34" spans="6:7">
-      <c r="F34" s="56"/>
+      <c r="F34" s="57"/>
     </row>
     <row r="35" spans="6:7">
-      <c r="F35" s="56"/>
+      <c r="F35" s="57"/>
     </row>
     <row r="36" spans="6:7">
-      <c r="F36" s="56"/>
+      <c r="F36" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5960,12 +7078,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF02F1A5-579B-6C4B-AE4C-80CB088C4869}">
   <dimension ref="C1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5998,14 +7116,14 @@
       </c>
       <c r="K3" s="55"/>
       <c r="L3" s="55"/>
-      <c r="M3" s="73"/>
+      <c r="M3" s="75"/>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
     </row>
     <row r="4" spans="3:15">
       <c r="K4" s="55"/>
       <c r="L4" s="55"/>
-      <c r="M4" s="73"/>
+      <c r="M4" s="75"/>
       <c r="N4" s="55"/>
       <c r="O4" s="55"/>
     </row>
@@ -6013,7 +7131,7 @@
       <c r="G5" s="22"/>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
-      <c r="M5" s="73"/>
+      <c r="M5" s="75"/>
       <c r="N5" s="55"/>
       <c r="O5" s="55"/>
     </row>
@@ -6021,7 +7139,7 @@
       <c r="G6" s="22"/>
       <c r="K6" s="55"/>
       <c r="L6" s="55"/>
-      <c r="M6" s="72" t="s">
+      <c r="M6" s="74" t="s">
         <v>63</v>
       </c>
       <c r="N6" s="55"/>
@@ -6031,7 +7149,7 @@
       <c r="G7" s="22"/>
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
-      <c r="M7" s="72"/>
+      <c r="M7" s="74"/>
       <c r="N7" s="55">
         <v>100</v>
       </c>
@@ -6041,7 +7159,7 @@
       <c r="G8" s="22"/>
       <c r="K8" s="55"/>
       <c r="L8" s="55"/>
-      <c r="M8" s="72"/>
+      <c r="M8" s="74"/>
       <c r="N8" s="55"/>
       <c r="O8" s="55"/>
     </row>
@@ -6052,7 +7170,7 @@
       <c r="G9" s="22"/>
       <c r="K9" s="55"/>
       <c r="L9" s="55"/>
-      <c r="M9" s="73"/>
+      <c r="M9" s="75"/>
       <c r="N9" s="55"/>
       <c r="O9" s="55"/>
     </row>
@@ -6065,7 +7183,7 @@
       </c>
       <c r="K10" s="55"/>
       <c r="L10" s="55"/>
-      <c r="M10" s="73"/>
+      <c r="M10" s="75"/>
       <c r="N10" s="55"/>
       <c r="O10" s="55"/>
     </row>
@@ -6077,10 +7195,10 @@
         <v>53</v>
       </c>
       <c r="K11" s="55"/>
-      <c r="L11" s="73" t="s">
+      <c r="L11" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="73"/>
+      <c r="M11" s="75"/>
       <c r="N11" s="55"/>
       <c r="O11" s="55"/>
     </row>
@@ -6159,7 +7277,7 @@
       </c>
     </row>
     <row r="22" spans="6:15">
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="69" t="s">
         <v>60</v>
       </c>
       <c r="H22" s="20" t="s">
@@ -6170,134 +7288,134 @@
       </c>
     </row>
     <row r="23" spans="6:15">
-      <c r="K23" s="69" t="s">
+      <c r="K23" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70" t="s">
+      <c r="L23" s="71"/>
+      <c r="M23" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
     </row>
     <row r="24" spans="6:15">
-      <c r="K24" s="68"/>
-      <c r="L24" s="72" t="s">
+      <c r="K24" s="70"/>
+      <c r="L24" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
     </row>
     <row r="25" spans="6:15">
-      <c r="K25" s="68"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
     </row>
     <row r="26" spans="6:15">
-      <c r="K26" s="71" t="s">
+      <c r="K26" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="L26" s="72"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
     </row>
     <row r="27" spans="6:15">
       <c r="G27" s="23"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="62"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
     </row>
     <row r="28" spans="6:15">
       <c r="G28" s="23"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="72" t="s">
+      <c r="K28" s="70"/>
+      <c r="L28" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
     </row>
     <row r="29" spans="6:15">
       <c r="F29" s="20" t="s">
         <v>40</v>
       </c>
       <c r="G29" s="23"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="62"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
     </row>
     <row r="30" spans="6:15">
       <c r="G30" s="23"/>
       <c r="H30" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="71" t="s">
+      <c r="K30" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="L30" s="72"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
     </row>
     <row r="31" spans="6:15">
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
     </row>
     <row r="32" spans="6:15">
       <c r="G32" s="23"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="62"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
     </row>
     <row r="33" spans="6:15">
       <c r="F33" s="20" t="s">
         <v>40</v>
       </c>
       <c r="G33" s="23"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
     </row>
     <row r="34" spans="6:15">
       <c r="G34" s="23"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="63"/>
     </row>
     <row r="35" spans="6:15">
       <c r="G35" s="23"/>
       <c r="H35" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="63"/>
     </row>
     <row r="36" spans="6:15">
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="63"/>
+      <c r="O36" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6311,17 +7429,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F003B54-18DF-4441-81E9-8E67CC05B6EF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] revice c language pointer for second two
</commit_message>
<xml_diff>
--- a/C内存图.xlsx
+++ b/C内存图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yytd/luochao/github_lc/c_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED98A5-DD65-A34A-AB93-18884CEFCAE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E607832-D461-A246-A770-A64991CFC115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17540" yWindow="2640" windowWidth="25200" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18220" yWindow="540" windowWidth="25200" windowHeight="16760" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="问答题" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
   <si>
     <t>1G（物理内存）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -532,7 +532,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">                                                                                          </t>
+    <t>不初始化，在栈上随机开辟的，地址指向的内荣不明确。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始化的时候设为NULL, 使用完毕设为NULL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5238,8 +5242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EDC0A7-B510-0D43-A3BA-720823ECA026}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5298,18 +5302,21 @@
       <c r="A11" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="82" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="12" spans="1:3" ht="30" customHeight="1">
       <c r="A12" s="82" t="s">
         <v>94</v>
       </c>
+      <c r="B12" s="82" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1">
       <c r="A13" s="82" t="s">
         <v>95</v>
+      </c>
+      <c r="B13" s="82" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" customHeight="1"/>
@@ -7266,7 +7273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF02F1A5-579B-6C4B-AE4C-80CB088C4869}">
   <dimension ref="C1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>

</xml_diff>